<commit_message>
proc/stat  get cpu and men show more than 100%
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="性能监控" sheetId="1" r:id="rId1"/>
     <sheet name="详细信息" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -32,7 +32,7 @@
     <t>网络</t>
   </si>
   <si>
-    <t>wifi</t>
+    <t>gprs</t>
   </si>
   <si>
     <t>耗时</t>
@@ -48,7 +48,7 @@
 </t>
   </si>
   <si>
-    <t>36秒</t>
+    <t>119秒</t>
   </si>
   <si>
     <t>CPU最大峰值</t>
@@ -87,31 +87,31 @@
     <t>下行流量均值</t>
   </si>
   <si>
-    <t>70.0%</t>
-  </si>
-  <si>
-    <t>39%</t>
-  </si>
-  <si>
-    <t>192M</t>
-  </si>
-  <si>
-    <t>52%</t>
-  </si>
-  <si>
-    <t>55.00</t>
-  </si>
-  <si>
-    <t>242KB</t>
-  </si>
-  <si>
-    <t>45KB</t>
-  </si>
-  <si>
-    <t>26KB</t>
-  </si>
-  <si>
-    <t>10KB</t>
+    <t>32%</t>
+  </si>
+  <si>
+    <t>6%</t>
+  </si>
+  <si>
+    <t>290M</t>
+  </si>
+  <si>
+    <t>92M</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>47KB</t>
+  </si>
+  <si>
+    <t>6KB</t>
+  </si>
+  <si>
+    <t>9KB</t>
+  </si>
+  <si>
+    <t>2KB</t>
   </si>
   <si>
     <t>cpu(%)</t>
@@ -136,11 +136,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -148,15 +148,8 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -197,15 +190,15 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -214,7 +207,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -246,81 +239,111 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$A$1:$A$16</c:f>
+              <c:f>详细信息!$A$1:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>61</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>61</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>61</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="141641216"/>
-        <c:axId val="141642752"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141641216"/>
+        <c:axId val="50010001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141642752"/>
+        <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141642752"/>
+        <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +351,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141641216"/>
+        <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -341,7 +364,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -349,7 +372,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -381,81 +404,111 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$B$1:$B$16</c:f>
+              <c:f>详细信息!$B$1:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>133</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>155</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>147</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>147</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>147</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>142</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>137</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>138</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>159</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>166</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>192</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>168</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>156</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>140</c:v>
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="163417088"/>
-        <c:axId val="163443456"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163417088"/>
+        <c:axId val="50020001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163443456"/>
+        <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163443456"/>
+        <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,7 +516,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163417088"/>
+        <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,7 +529,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -484,7 +537,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -516,87 +569,117 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$D$1:$D$18</c:f>
+              <c:f>详细信息!$D$1:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>90</c:v>
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="165298560"/>
-        <c:axId val="165300096"/>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165298560"/>
+        <c:axId val="50030001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165300096"/>
+        <c:crossAx val="50030002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165300096"/>
+        <c:axId val="50030002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +687,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165298560"/>
+        <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -617,7 +700,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -625,7 +708,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -657,24 +740,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$C$1:$C$16</c:f>
+              <c:f>详细信息!$C$1:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>60</c:v>
@@ -686,27 +769,57 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>52</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
@@ -714,24 +827,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="165328384"/>
-        <c:axId val="165329920"/>
+        <c:axId val="50040001"/>
+        <c:axId val="50040002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165328384"/>
+        <c:axId val="50040001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165329920"/>
+        <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165329920"/>
+        <c:axId val="50040002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +852,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165328384"/>
+        <c:crossAx val="50040001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -752,7 +865,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -760,7 +873,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -778,14 +891,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.37427434116860847"/>
-          <c:y val="3.0769230769230771E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -799,81 +905,111 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$E$1:$E$16</c:f>
+              <c:f>详细信息!$E$1:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10650</c:v>
+                  <c:v>149006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10891</c:v>
+                  <c:v>149053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10891</c:v>
+                  <c:v>149090</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11015</c:v>
+                  <c:v>149093</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11015</c:v>
+                  <c:v>149093</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11015</c:v>
+                  <c:v>149095</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11019</c:v>
+                  <c:v>149101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11038</c:v>
+                  <c:v>149102</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11055</c:v>
+                  <c:v>149102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11203</c:v>
+                  <c:v>149103</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11245</c:v>
+                  <c:v>149104</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11245</c:v>
+                  <c:v>149104</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11249</c:v>
+                  <c:v>149104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11264</c:v>
+                  <c:v>149105</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11276</c:v>
+                  <c:v>149105</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>149105</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>149105</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>149133</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>149133</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>149145</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>149145</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>149145</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>149145</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>149150</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>149150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166664832"/>
-        <c:axId val="166670720"/>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166664832"/>
+        <c:axId val="50050001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166670720"/>
+        <c:crossAx val="50050002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166670720"/>
+        <c:axId val="50050002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +1017,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166664832"/>
+        <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -894,7 +1030,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -902,7 +1038,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -934,81 +1070,111 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>详细信息!$F$1:$F$16</c:f>
+              <c:f>详细信息!$F$1:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1734</c:v>
+                  <c:v>17937</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1759</c:v>
+                  <c:v>17941</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1760</c:v>
+                  <c:v>17942</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1776</c:v>
+                  <c:v>17946</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1776</c:v>
+                  <c:v>17946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1777</c:v>
+                  <c:v>17946</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1780</c:v>
+                  <c:v>17947</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1793</c:v>
+                  <c:v>17947</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1809</c:v>
+                  <c:v>17947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1826</c:v>
+                  <c:v>17948</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1835</c:v>
+                  <c:v>17948</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1835</c:v>
+                  <c:v>17948</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1843</c:v>
+                  <c:v>17950</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1855</c:v>
+                  <c:v>17950</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1867</c:v>
+                  <c:v>17951</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17951</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17951</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17961</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17967</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17967</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17967</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17967</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17969</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166715392"/>
-        <c:axId val="166716928"/>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166715392"/>
+        <c:axId val="50060001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166716928"/>
+        <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166716928"/>
+        <c:axId val="50060002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,7 +1182,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166715392"/>
+        <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1029,7 +1195,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1041,14 +1207,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1069,16 +1235,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1099,16 +1265,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1129,16 +1295,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1159,16 +1325,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1189,16 +1355,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1221,7 +1387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1507,137 +1673,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
-    <col min="2" max="12" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="1">
-        <v>90</v>
-      </c>
-      <c r="H4" s="1">
-        <v>90</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G4" s="2">
+        <v>93</v>
+      </c>
+      <c r="H4" s="2">
+        <v>93</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1654,355 +1828,557 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
-      <c r="A2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>133</v>
-      </c>
-      <c r="C2" s="1">
-        <v>55</v>
-      </c>
-      <c r="D2" s="1">
-        <v>89</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10650</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1734</v>
+      <c r="A2" s="2">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2">
+        <v>262</v>
+      </c>
+      <c r="C2" s="2">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2">
+        <v>92</v>
+      </c>
+      <c r="E2" s="2">
+        <v>149006</v>
+      </c>
+      <c r="F2" s="2">
+        <v>17937</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="A3" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>155</v>
-      </c>
-      <c r="C3" s="1">
-        <v>48</v>
-      </c>
-      <c r="D3" s="1">
-        <v>89</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10891</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1759</v>
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>290</v>
+      </c>
+      <c r="C3" s="2">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2">
+        <v>92</v>
+      </c>
+      <c r="E3" s="2">
+        <v>149053</v>
+      </c>
+      <c r="F3" s="2">
+        <v>17941</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
-      <c r="A4" s="1">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1">
-        <v>147</v>
-      </c>
-      <c r="C4" s="1">
-        <v>56</v>
-      </c>
-      <c r="D4" s="1">
-        <v>89</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10891</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1760</v>
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>266</v>
+      </c>
+      <c r="C4" s="2">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2">
+        <v>92</v>
+      </c>
+      <c r="E4" s="2">
+        <v>149090</v>
+      </c>
+      <c r="F4" s="2">
+        <v>17942</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1">
-      <c r="A5" s="1">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
-        <v>149</v>
-      </c>
-      <c r="C5" s="1">
-        <v>57</v>
-      </c>
-      <c r="D5" s="1">
-        <v>90</v>
-      </c>
-      <c r="E5" s="1">
-        <v>11015</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1776</v>
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>267</v>
+      </c>
+      <c r="C5" s="2">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2">
+        <v>92</v>
+      </c>
+      <c r="E5" s="2">
+        <v>149093</v>
+      </c>
+      <c r="F5" s="2">
+        <v>17946</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="1">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1">
-        <v>147</v>
-      </c>
-      <c r="C6" s="1">
-        <v>60</v>
-      </c>
-      <c r="D6" s="1">
-        <v>90</v>
-      </c>
-      <c r="E6" s="1">
-        <v>11015</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1776</v>
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>268</v>
+      </c>
+      <c r="C6" s="2">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2">
+        <v>92</v>
+      </c>
+      <c r="E6" s="2">
+        <v>149093</v>
+      </c>
+      <c r="F6" s="2">
+        <v>17946</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1">
-      <c r="A7" s="1">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1">
-        <v>147</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60</v>
-      </c>
-      <c r="D7" s="1">
-        <v>90</v>
-      </c>
-      <c r="E7" s="1">
-        <v>11015</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1777</v>
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>271</v>
+      </c>
+      <c r="C7" s="2">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2">
+        <v>92</v>
+      </c>
+      <c r="E7" s="2">
+        <v>149095</v>
+      </c>
+      <c r="F7" s="2">
+        <v>17946</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1">
-        <v>142</v>
-      </c>
-      <c r="C8" s="1">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1">
-        <v>90</v>
-      </c>
-      <c r="E8" s="1">
-        <v>11019</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1780</v>
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>266</v>
+      </c>
+      <c r="C8" s="2">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2">
+        <v>92</v>
+      </c>
+      <c r="E8" s="2">
+        <v>149101</v>
+      </c>
+      <c r="F8" s="2">
+        <v>17947</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>43</v>
-      </c>
-      <c r="B9" s="1">
-        <v>137</v>
-      </c>
-      <c r="C9" s="1">
-        <v>55</v>
-      </c>
-      <c r="D9" s="1">
-        <v>90</v>
-      </c>
-      <c r="E9" s="1">
-        <v>11038</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1793</v>
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>271</v>
+      </c>
+      <c r="C9" s="2">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2">
+        <v>92</v>
+      </c>
+      <c r="E9" s="2">
+        <v>149102</v>
+      </c>
+      <c r="F9" s="2">
+        <v>17947</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1">
-        <v>138</v>
-      </c>
-      <c r="C10" s="1">
-        <v>53</v>
-      </c>
-      <c r="D10" s="1">
-        <v>90</v>
-      </c>
-      <c r="E10" s="1">
-        <v>11055</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1809</v>
+      <c r="A10" s="2">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>271</v>
+      </c>
+      <c r="C10" s="2">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2">
+        <v>92</v>
+      </c>
+      <c r="E10" s="2">
+        <v>149102</v>
+      </c>
+      <c r="F10" s="2">
+        <v>17947</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1">
-        <v>159</v>
-      </c>
-      <c r="C11" s="1">
-        <v>56</v>
-      </c>
-      <c r="D11" s="1">
-        <v>90</v>
-      </c>
-      <c r="E11" s="1">
-        <v>11203</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1826</v>
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>252</v>
+      </c>
+      <c r="C11" s="2">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2">
+        <v>92</v>
+      </c>
+      <c r="E11" s="2">
+        <v>149103</v>
+      </c>
+      <c r="F11" s="2">
+        <v>17948</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>70</v>
-      </c>
-      <c r="B12" s="1">
-        <v>166</v>
-      </c>
-      <c r="C12" s="1">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1">
-        <v>90</v>
-      </c>
-      <c r="E12" s="1">
-        <v>11245</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1835</v>
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>248</v>
+      </c>
+      <c r="C12" s="2">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2">
+        <v>92</v>
+      </c>
+      <c r="E12" s="2">
+        <v>149104</v>
+      </c>
+      <c r="F12" s="2">
+        <v>17948</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>70</v>
-      </c>
-      <c r="B13" s="1">
-        <v>192</v>
-      </c>
-      <c r="C13" s="1">
-        <v>52</v>
-      </c>
-      <c r="D13" s="1">
-        <v>90</v>
-      </c>
-      <c r="E13" s="1">
-        <v>11245</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1835</v>
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>265</v>
+      </c>
+      <c r="C13" s="2">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2">
+        <v>92</v>
+      </c>
+      <c r="E13" s="2">
+        <v>149104</v>
+      </c>
+      <c r="F13" s="2">
+        <v>17948</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>61</v>
-      </c>
-      <c r="B14" s="1">
-        <v>168</v>
-      </c>
-      <c r="C14" s="1">
-        <v>50</v>
-      </c>
-      <c r="D14" s="1">
-        <v>90</v>
-      </c>
-      <c r="E14" s="1">
-        <v>11249</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1843</v>
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>262</v>
+      </c>
+      <c r="C14" s="2">
+        <v>60</v>
+      </c>
+      <c r="D14" s="2">
+        <v>92</v>
+      </c>
+      <c r="E14" s="2">
+        <v>149104</v>
+      </c>
+      <c r="F14" s="2">
+        <v>17950</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>61</v>
-      </c>
-      <c r="B15" s="1">
-        <v>156</v>
-      </c>
-      <c r="C15" s="1">
-        <v>57</v>
-      </c>
-      <c r="D15" s="1">
-        <v>90</v>
-      </c>
-      <c r="E15" s="1">
-        <v>11264</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1855</v>
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>260</v>
+      </c>
+      <c r="C15" s="2">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2">
+        <v>92</v>
+      </c>
+      <c r="E15" s="2">
+        <v>149105</v>
+      </c>
+      <c r="F15" s="2">
+        <v>17950</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1">
-        <v>140</v>
-      </c>
-      <c r="C16" s="1">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1">
-        <v>90</v>
-      </c>
-      <c r="E16" s="1">
-        <v>11276</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1867</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="1">
-        <v>90</v>
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>264</v>
+      </c>
+      <c r="C16" s="2">
+        <v>60</v>
+      </c>
+      <c r="D16" s="2">
+        <v>92</v>
+      </c>
+      <c r="E16" s="2">
+        <v>149105</v>
+      </c>
+      <c r="F16" s="2">
+        <v>17951</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>259</v>
+      </c>
+      <c r="C17" s="2">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2">
+        <v>92</v>
+      </c>
+      <c r="E17" s="2">
+        <v>149105</v>
+      </c>
+      <c r="F17" s="2">
+        <v>17951</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>252</v>
+      </c>
+      <c r="C18" s="2">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2">
+        <v>93</v>
+      </c>
+      <c r="E18" s="2">
+        <v>149105</v>
+      </c>
+      <c r="F18" s="2">
+        <v>17951</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>251</v>
+      </c>
+      <c r="C19" s="2">
+        <v>60</v>
+      </c>
+      <c r="D19" s="2">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2">
+        <v>149133</v>
+      </c>
+      <c r="F19" s="2">
+        <v>17959</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2">
+        <v>268</v>
+      </c>
+      <c r="C20" s="2">
+        <v>60</v>
+      </c>
+      <c r="D20" s="2">
+        <v>93</v>
+      </c>
+      <c r="E20" s="2">
+        <v>149133</v>
+      </c>
+      <c r="F20" s="2">
+        <v>17961</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2">
+        <v>282</v>
+      </c>
+      <c r="C21" s="2">
+        <v>60</v>
+      </c>
+      <c r="D21" s="2">
+        <v>93</v>
+      </c>
+      <c r="E21" s="2">
+        <v>149145</v>
+      </c>
+      <c r="F21" s="2">
+        <v>17967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2">
+        <v>279</v>
+      </c>
+      <c r="C22" s="2">
+        <v>60</v>
+      </c>
+      <c r="D22" s="2">
+        <v>93</v>
+      </c>
+      <c r="E22" s="2">
+        <v>149145</v>
+      </c>
+      <c r="F22" s="2">
+        <v>17967</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2">
+        <v>280</v>
+      </c>
+      <c r="C23" s="2">
+        <v>60</v>
+      </c>
+      <c r="D23" s="2">
+        <v>93</v>
+      </c>
+      <c r="E23" s="2">
+        <v>149145</v>
+      </c>
+      <c r="F23" s="2">
+        <v>17967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2">
+        <v>280</v>
+      </c>
+      <c r="C24" s="2">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2">
+        <v>93</v>
+      </c>
+      <c r="E24" s="2">
+        <v>149145</v>
+      </c>
+      <c r="F24" s="2">
+        <v>17967</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2">
+        <v>281</v>
+      </c>
+      <c r="C25" s="2">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2">
+        <v>93</v>
+      </c>
+      <c r="E25" s="2">
+        <v>149150</v>
+      </c>
+      <c r="F25" s="2">
+        <v>17969</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2">
+        <v>281</v>
+      </c>
+      <c r="C26" s="2">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2">
+        <v>93</v>
+      </c>
+      <c r="E26" s="2">
+        <v>149150</v>
+      </c>
+      <c r="F26" s="2">
+        <v>17969</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="D27" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="D28" s="2">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>